<commit_message>
Acutalizacion de Utilidades sin campo nuevo
</commit_message>
<xml_diff>
--- a/uploads/CategoriaNuevo/CategoriaMinaPanulcillo.xlsx
+++ b/uploads/CategoriaNuevo/CategoriaMinaPanulcillo.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/CategoriaNuevo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78646972-F38B-434F-8DB7-8B3DC94AE24C}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E7138CE-EEA2-4274-9290-D392951DF741}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>id</t>
   </si>
@@ -265,6 +276,9 @@
   </si>
   <si>
     <t>Informe Consolidado Final del Proyecto</t>
+  </si>
+  <si>
+    <t>Utilidades</t>
   </si>
 </sst>
 </file>
@@ -547,8 +561,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}" name="Tabla1" displayName="Tabla1" ref="A1:G74" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:G74" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}" name="Tabla1" displayName="Tabla1" ref="A1:G75" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:G75" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{115A9EBB-5BAD-4271-B80E-885F0DCBFFF7}" name="id"/>
     <tableColumn id="2" xr3:uid="{90C47675-E299-400A-B78E-8C89E0E72C69}" name="nombre" dataDxfId="0"/>
@@ -825,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:XFD53"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2532,6 +2546,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="21">
+        <v>44071</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="E75" s="21">
+        <v>44071</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Actualizacion campo MB de tabla GestionPermisos
</commit_message>
<xml_diff>
--- a/uploads/CategoriaNuevo/CategoriaMinaPanulcillo.xlsx
+++ b/uploads/CategoriaNuevo/CategoriaMinaPanulcillo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/CategoriaNuevo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E7138CE-EEA2-4274-9290-D392951DF741}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1320D883-B4B7-4E1C-AFB0-16D9ADF68BF0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -841,15 +841,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="75.36328125" customWidth="1"/>
-    <col min="3" max="4" width="10.26953125" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Actualizacion Filtro Proyecto en tablas
</commit_message>
<xml_diff>
--- a/uploads/CategoriaNuevo/CategoriaMinaPanulcillo.xlsx
+++ b/uploads/CategoriaNuevo/CategoriaMinaPanulcillo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enami-my.sharepoint.com/personal/pjdiaz_enami_cl/Documents/Escritorio/Proyecto37/Proyecto16/Proyecto11/proyecto2/uploads/CategoriaNuevo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1320D883-B4B7-4E1C-AFB0-16D9ADF68BF0}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="11_AD4D2F04E46CFB4ACB3E20C07D90DEBA683EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87A9F6AB-5458-4359-98BE-4886601B5490}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>id</t>
   </si>
@@ -279,6 +279,90 @@
   </si>
   <si>
     <t>Utilidades</t>
+  </si>
+  <si>
+    <t>Maquinaria Costo Directo</t>
+  </si>
+  <si>
+    <t>BULLDOZER 20 TON</t>
+  </si>
+  <si>
+    <t>CAMION ALJIBE 30 M3</t>
+  </si>
+  <si>
+    <t>CAMION GRUA 12 TON</t>
+  </si>
+  <si>
+    <t>CAMION TOLVA 20 M3</t>
+  </si>
+  <si>
+    <t>EXCAVADORA 20 T</t>
+  </si>
+  <si>
+    <t>GRÚA HIDRÁULICA 60 TON</t>
+  </si>
+  <si>
+    <t>MINICARGADOR 3 TON</t>
+  </si>
+  <si>
+    <t>MOTONIVELADORA 18 TON</t>
+  </si>
+  <si>
+    <t>PLACA COMPACTADORA 80 KG</t>
+  </si>
+  <si>
+    <t>RETROEXCAVADORA 8 TON</t>
+  </si>
+  <si>
+    <t>RODILLO COMPACTADOR 12 TON</t>
+  </si>
+  <si>
+    <t>RODILLO DOBLE TAMBOR MANUAL</t>
+  </si>
+  <si>
+    <t>AYUDANTE</t>
+  </si>
+  <si>
+    <t>CAPATAZ</t>
+  </si>
+  <si>
+    <t>MAESTRO 1ERA</t>
+  </si>
+  <si>
+    <t>MAESTRO 2DA</t>
+  </si>
+  <si>
+    <t>OPERADOR BULLDOZER</t>
+  </si>
+  <si>
+    <t>OPERADOR CAMIÓN PLUMA</t>
+  </si>
+  <si>
+    <t>OPERADOR CAMIÓN TOLVA</t>
+  </si>
+  <si>
+    <t>OPERADOR CAMIÓN ALJIBE</t>
+  </si>
+  <si>
+    <t>OPERADOR DE RETROEXCAVADORA</t>
+  </si>
+  <si>
+    <t>OPERADOR EXCAVADORA</t>
+  </si>
+  <si>
+    <t>OPERADOR MOTONIVELADORA</t>
+  </si>
+  <si>
+    <t>OPERADOR MINICARGADOR</t>
+  </si>
+  <si>
+    <t>OPERADOR RODILLO COMPACTADOR</t>
+  </si>
+  <si>
+    <t>RIGGER</t>
+  </si>
+  <si>
+    <t>Mano Obra Costo Directo</t>
   </si>
 </sst>
 </file>
@@ -420,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -467,6 +551,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,16 +591,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -561,8 +646,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}" name="Tabla1" displayName="Tabla1" ref="A1:G75" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:G75" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}" name="Tabla1" displayName="Tabla1" ref="A1:G103" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:G103" xr:uid="{B6D47527-3F8D-4421-BFB1-FD8B877FFD7B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{115A9EBB-5BAD-4271-B80E-885F0DCBFFF7}" name="id"/>
     <tableColumn id="2" xr3:uid="{90C47675-E299-400A-B78E-8C89E0E72C69}" name="nombre" dataDxfId="0"/>
@@ -839,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2567,6 +2652,645 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="18">
+        <v>44072</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="E76" s="18">
+        <v>44072</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="21">
+        <v>44073</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77">
+        <v>5</v>
+      </c>
+      <c r="D77">
+        <v>44072</v>
+      </c>
+      <c r="E77" s="21">
+        <v>44073</v>
+      </c>
+      <c r="F77">
+        <v>2</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="18">
+        <v>44074</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78">
+        <v>5</v>
+      </c>
+      <c r="D78">
+        <v>44072</v>
+      </c>
+      <c r="E78" s="18">
+        <v>44074</v>
+      </c>
+      <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="21">
+        <v>44075</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79">
+        <v>44072</v>
+      </c>
+      <c r="E79" s="21">
+        <v>44075</v>
+      </c>
+      <c r="F79">
+        <v>2</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="18">
+        <v>44076</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80">
+        <v>5</v>
+      </c>
+      <c r="D80">
+        <v>44072</v>
+      </c>
+      <c r="E80" s="18">
+        <v>44076</v>
+      </c>
+      <c r="F80">
+        <v>2</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="21">
+        <v>44077</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>44072</v>
+      </c>
+      <c r="E81" s="21">
+        <v>44077</v>
+      </c>
+      <c r="F81">
+        <v>2</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="18">
+        <v>44078</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82">
+        <v>44072</v>
+      </c>
+      <c r="E82" s="18">
+        <v>44078</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="21">
+        <v>44079</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <v>44072</v>
+      </c>
+      <c r="E83" s="21">
+        <v>44079</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="18">
+        <v>44080</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+      <c r="D84">
+        <v>44072</v>
+      </c>
+      <c r="E84" s="18">
+        <v>44080</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="21">
+        <v>44081</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>44072</v>
+      </c>
+      <c r="E85" s="21">
+        <v>44081</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="18">
+        <v>44082</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>44072</v>
+      </c>
+      <c r="E86" s="18">
+        <v>44082</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="21">
+        <v>44083</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
+      </c>
+      <c r="D87">
+        <v>44072</v>
+      </c>
+      <c r="E87" s="21">
+        <v>44083</v>
+      </c>
+      <c r="F87">
+        <v>2</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="18">
+        <v>44084</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>44072</v>
+      </c>
+      <c r="E88" s="18">
+        <v>44084</v>
+      </c>
+      <c r="F88">
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="21">
+        <v>44085</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E89" s="21">
+        <v>44085</v>
+      </c>
+      <c r="F89" s="24">
+        <v>2</v>
+      </c>
+      <c r="G89" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="18">
+        <v>44086</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E90" s="18">
+        <v>44086</v>
+      </c>
+      <c r="F90" s="24">
+        <v>2</v>
+      </c>
+      <c r="G90" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="21">
+        <v>44087</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+      <c r="D91" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E91" s="21">
+        <v>44087</v>
+      </c>
+      <c r="F91" s="24">
+        <v>2</v>
+      </c>
+      <c r="G91" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="18">
+        <v>44088</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="D92" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E92" s="18">
+        <v>44088</v>
+      </c>
+      <c r="F92" s="24">
+        <v>2</v>
+      </c>
+      <c r="G92" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="21">
+        <v>44089</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+      <c r="D93" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E93" s="21">
+        <v>44089</v>
+      </c>
+      <c r="F93" s="24">
+        <v>2</v>
+      </c>
+      <c r="G93" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="18">
+        <v>44090</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+      <c r="D94" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E94" s="18">
+        <v>44090</v>
+      </c>
+      <c r="F94" s="24">
+        <v>2</v>
+      </c>
+      <c r="G94" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="21">
+        <v>44091</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C95">
+        <v>5</v>
+      </c>
+      <c r="D95" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E95" s="21">
+        <v>44091</v>
+      </c>
+      <c r="F95" s="24">
+        <v>2</v>
+      </c>
+      <c r="G95" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="18">
+        <v>44092</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="D96" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E96" s="18">
+        <v>44092</v>
+      </c>
+      <c r="F96" s="24">
+        <v>2</v>
+      </c>
+      <c r="G96" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="21">
+        <v>44093</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
+      </c>
+      <c r="D97" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E97" s="21">
+        <v>44093</v>
+      </c>
+      <c r="F97" s="24">
+        <v>2</v>
+      </c>
+      <c r="G97" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="18">
+        <v>44094</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C98">
+        <v>5</v>
+      </c>
+      <c r="D98" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E98" s="18">
+        <v>44094</v>
+      </c>
+      <c r="F98" s="24">
+        <v>2</v>
+      </c>
+      <c r="G98" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="21">
+        <v>44095</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+      <c r="D99" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E99" s="21">
+        <v>44095</v>
+      </c>
+      <c r="F99" s="24">
+        <v>2</v>
+      </c>
+      <c r="G99" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="18">
+        <v>44096</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C100">
+        <v>5</v>
+      </c>
+      <c r="D100" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E100" s="18">
+        <v>44096</v>
+      </c>
+      <c r="F100" s="24">
+        <v>2</v>
+      </c>
+      <c r="G100" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="21">
+        <v>44097</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+      <c r="D101" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E101" s="21">
+        <v>44097</v>
+      </c>
+      <c r="F101" s="24">
+        <v>2</v>
+      </c>
+      <c r="G101" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="18">
+        <v>44098</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+      <c r="D102" s="24">
+        <v>44099</v>
+      </c>
+      <c r="E102" s="18">
+        <v>44098</v>
+      </c>
+      <c r="F102" s="24">
+        <v>2</v>
+      </c>
+      <c r="G102" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="21">
+        <v>44099</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" s="24">
+        <v>5</v>
+      </c>
+      <c r="D103" s="24"/>
+      <c r="E103" s="21">
+        <v>44099</v>
+      </c>
+      <c r="F103" s="24">
+        <v>1</v>
+      </c>
+      <c r="G103" s="24">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>